<commit_message>
testing for rolling_agg funcs, refreshed stock label data; replaced 6m period with 3m
</commit_message>
<xml_diff>
--- a/ml/stock_data/buy_sell_labels/DOW.xlsx
+++ b/ml/stock_data/buy_sell_labels/DOW.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C168"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,10 +387,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43802</v>
+        <v>43707</v>
       </c>
       <c r="C2" t="n">
-        <v>50.08</v>
+        <v>40.68</v>
       </c>
     </row>
     <row r="3">
@@ -398,10 +398,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43803</v>
+        <v>43711</v>
       </c>
       <c r="C3" t="n">
-        <v>50.53</v>
+        <v>39.89</v>
       </c>
     </row>
     <row r="4">
@@ -409,10 +409,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43804</v>
+        <v>43712</v>
       </c>
       <c r="C4" t="n">
-        <v>50.26</v>
+        <v>40.59</v>
       </c>
     </row>
     <row r="5">
@@ -420,10 +420,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43805</v>
+        <v>43713</v>
       </c>
       <c r="C5" t="n">
-        <v>51.43</v>
+        <v>41.38</v>
       </c>
     </row>
     <row r="6">
@@ -431,10 +431,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43808</v>
+        <v>43714</v>
       </c>
       <c r="C6" t="n">
-        <v>51.48</v>
+        <v>41.26</v>
       </c>
     </row>
     <row r="7">
@@ -442,10 +442,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>43809</v>
+        <v>43717</v>
       </c>
       <c r="C7" t="n">
-        <v>51.35</v>
+        <v>42.42</v>
       </c>
     </row>
     <row r="8">
@@ -453,10 +453,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43810</v>
+        <v>43718</v>
       </c>
       <c r="C8" t="n">
-        <v>51.32</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="9">
@@ -464,10 +464,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>43811</v>
+        <v>43719</v>
       </c>
       <c r="C9" t="n">
-        <v>52.62</v>
+        <v>44.73</v>
       </c>
     </row>
     <row r="10">
@@ -475,10 +475,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>43812</v>
+        <v>43720</v>
       </c>
       <c r="C10" t="n">
-        <v>51.49</v>
+        <v>44.82</v>
       </c>
     </row>
     <row r="11">
@@ -486,10 +486,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43815</v>
+        <v>43721</v>
       </c>
       <c r="C11" t="n">
-        <v>52.35</v>
+        <v>45.99</v>
       </c>
     </row>
     <row r="12">
@@ -497,10 +497,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>43816</v>
+        <v>43724</v>
       </c>
       <c r="C12" t="n">
-        <v>52.83</v>
+        <v>46.77</v>
       </c>
     </row>
     <row r="13">
@@ -508,10 +508,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>43817</v>
+        <v>43725</v>
       </c>
       <c r="C13" t="n">
-        <v>52.43</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="14">
@@ -519,10 +519,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>43818</v>
+        <v>43726</v>
       </c>
       <c r="C14" t="n">
-        <v>52.69</v>
+        <v>45.34</v>
       </c>
     </row>
     <row r="15">
@@ -530,10 +530,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>43819</v>
+        <v>43727</v>
       </c>
       <c r="C15" t="n">
-        <v>52.78</v>
+        <v>45.46</v>
       </c>
     </row>
     <row r="16">
@@ -541,10 +541,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>43822</v>
+        <v>43728</v>
       </c>
       <c r="C16" t="n">
-        <v>53.09</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17">
@@ -552,10 +552,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>43823</v>
+        <v>43731</v>
       </c>
       <c r="C17" t="n">
-        <v>53.06</v>
+        <v>45.72</v>
       </c>
     </row>
     <row r="18">
@@ -563,10 +563,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>43825</v>
+        <v>43732</v>
       </c>
       <c r="C18" t="n">
-        <v>53.37</v>
+        <v>44.47</v>
       </c>
     </row>
     <row r="19">
@@ -574,10 +574,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>43826</v>
+        <v>43733</v>
       </c>
       <c r="C19" t="n">
-        <v>52.99</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="20">
@@ -585,10 +585,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>43829</v>
+        <v>43734</v>
       </c>
       <c r="C20" t="n">
-        <v>52.52</v>
+        <v>45.07</v>
       </c>
     </row>
     <row r="21">
@@ -596,10 +596,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>43830</v>
+        <v>43735</v>
       </c>
       <c r="C21" t="n">
-        <v>52.89</v>
+        <v>44.92</v>
       </c>
     </row>
     <row r="22">
@@ -607,10 +607,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>43832</v>
+        <v>43738</v>
       </c>
       <c r="C22" t="n">
-        <v>51.95</v>
+        <v>45.47</v>
       </c>
     </row>
     <row r="23">
@@ -618,10 +618,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>43833</v>
+        <v>43739</v>
       </c>
       <c r="C23" t="n">
-        <v>50.66</v>
+        <v>43.87</v>
       </c>
     </row>
     <row r="24">
@@ -629,10 +629,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>43836</v>
+        <v>43740</v>
       </c>
       <c r="C24" t="n">
-        <v>50.46</v>
+        <v>42.87</v>
       </c>
     </row>
     <row r="25">
@@ -640,10 +640,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>43837</v>
+        <v>43741</v>
       </c>
       <c r="C25" t="n">
-        <v>50.44</v>
+        <v>43.24</v>
       </c>
     </row>
     <row r="26">
@@ -651,10 +651,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>43838</v>
+        <v>43742</v>
       </c>
       <c r="C26" t="n">
-        <v>50.96</v>
+        <v>43.26</v>
       </c>
     </row>
     <row r="27">
@@ -662,10 +662,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>43839</v>
+        <v>43745</v>
       </c>
       <c r="C27" t="n">
-        <v>50.44</v>
+        <v>43.1</v>
       </c>
     </row>
     <row r="28">
@@ -673,10 +673,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>43840</v>
+        <v>43746</v>
       </c>
       <c r="C28" t="n">
-        <v>49.77</v>
+        <v>41.84</v>
       </c>
     </row>
     <row r="29">
@@ -684,10 +684,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>43843</v>
+        <v>43747</v>
       </c>
       <c r="C29" t="n">
-        <v>50.59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30">
@@ -695,10 +695,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>43844</v>
+        <v>43748</v>
       </c>
       <c r="C30" t="n">
-        <v>50.49</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="31">
@@ -706,10 +706,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>43845</v>
+        <v>43749</v>
       </c>
       <c r="C31" t="n">
-        <v>50.52</v>
+        <v>44.97</v>
       </c>
     </row>
     <row r="32">
@@ -717,10 +717,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>43846</v>
+        <v>43752</v>
       </c>
       <c r="C32" t="n">
-        <v>50.72</v>
+        <v>44.68</v>
       </c>
     </row>
     <row r="33">
@@ -728,10 +728,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>43847</v>
+        <v>43753</v>
       </c>
       <c r="C33" t="n">
-        <v>51.55</v>
+        <v>45.04</v>
       </c>
     </row>
     <row r="34">
@@ -739,10 +739,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>43851</v>
+        <v>43754</v>
       </c>
       <c r="C34" t="n">
-        <v>50.84</v>
+        <v>44.96</v>
       </c>
     </row>
     <row r="35">
@@ -750,10 +750,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>43852</v>
+        <v>43755</v>
       </c>
       <c r="C35" t="n">
-        <v>49.16</v>
+        <v>45.62</v>
       </c>
     </row>
     <row r="36">
@@ -761,10 +761,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>43853</v>
+        <v>43756</v>
       </c>
       <c r="C36" t="n">
-        <v>48.56</v>
+        <v>45.76</v>
       </c>
     </row>
     <row r="37">
@@ -772,10 +772,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>43854</v>
+        <v>43759</v>
       </c>
       <c r="C37" t="n">
-        <v>46.86</v>
+        <v>44.96</v>
       </c>
     </row>
     <row r="38">
@@ -783,10 +783,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>43857</v>
+        <v>43760</v>
       </c>
       <c r="C38" t="n">
-        <v>45.6</v>
+        <v>44.68</v>
       </c>
     </row>
     <row r="39">
@@ -794,10 +794,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>43858</v>
+        <v>43761</v>
       </c>
       <c r="C39" t="n">
-        <v>45.58</v>
+        <v>45.07</v>
       </c>
     </row>
     <row r="40">
@@ -805,10 +805,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>43859</v>
+        <v>43762</v>
       </c>
       <c r="C40" t="n">
-        <v>48</v>
+        <v>47.21</v>
       </c>
     </row>
     <row r="41">
@@ -816,10 +816,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>43860</v>
+        <v>43763</v>
       </c>
       <c r="C41" t="n">
-        <v>46.84</v>
+        <v>48.17</v>
       </c>
     </row>
     <row r="42">
@@ -827,10 +827,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>43861</v>
+        <v>43766</v>
       </c>
       <c r="C42" t="n">
-        <v>44.52</v>
+        <v>48.87</v>
       </c>
     </row>
     <row r="43">
@@ -838,10 +838,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>43864</v>
+        <v>43767</v>
       </c>
       <c r="C43" t="n">
-        <v>45.17</v>
+        <v>49.13</v>
       </c>
     </row>
     <row r="44">
@@ -849,10 +849,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>43865</v>
+        <v>43768</v>
       </c>
       <c r="C44" t="n">
-        <v>46.44</v>
+        <v>48.69</v>
       </c>
     </row>
     <row r="45">
@@ -860,10 +860,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>43866</v>
+        <v>43769</v>
       </c>
       <c r="C45" t="n">
-        <v>47.95</v>
+        <v>48.18</v>
       </c>
     </row>
     <row r="46">
@@ -871,10 +871,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>43867</v>
+        <v>43770</v>
       </c>
       <c r="C46" t="n">
-        <v>47.55</v>
+        <v>49.92</v>
       </c>
     </row>
     <row r="47">
@@ -882,10 +882,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>43868</v>
+        <v>43773</v>
       </c>
       <c r="C47" t="n">
-        <v>46.42</v>
+        <v>51.69</v>
       </c>
     </row>
     <row r="48">
@@ -893,10 +893,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>43871</v>
+        <v>43774</v>
       </c>
       <c r="C48" t="n">
-        <v>46.57</v>
+        <v>51.72</v>
       </c>
     </row>
     <row r="49">
@@ -904,10 +904,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>43872</v>
+        <v>43775</v>
       </c>
       <c r="C49" t="n">
-        <v>47.15</v>
+        <v>51.8</v>
       </c>
     </row>
     <row r="50">
@@ -915,10 +915,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>43873</v>
+        <v>43776</v>
       </c>
       <c r="C50" t="n">
-        <v>47.72</v>
+        <v>53.25</v>
       </c>
     </row>
     <row r="51">
@@ -926,10 +926,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>43874</v>
+        <v>43777</v>
       </c>
       <c r="C51" t="n">
-        <v>46.68</v>
+        <v>53.43</v>
       </c>
     </row>
     <row r="52">
@@ -937,10 +937,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>43875</v>
+        <v>43780</v>
       </c>
       <c r="C52" t="n">
-        <v>47</v>
+        <v>53.26</v>
       </c>
     </row>
     <row r="53">
@@ -948,10 +948,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>43879</v>
+        <v>43781</v>
       </c>
       <c r="C53" t="n">
-        <v>46.14</v>
+        <v>52.64</v>
       </c>
     </row>
     <row r="54">
@@ -959,10 +959,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>43880</v>
+        <v>43782</v>
       </c>
       <c r="C54" t="n">
-        <v>45.96</v>
+        <v>51.2</v>
       </c>
     </row>
     <row r="55">
@@ -970,10 +970,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>43881</v>
+        <v>43783</v>
       </c>
       <c r="C55" t="n">
-        <v>47.12</v>
+        <v>51.48</v>
       </c>
     </row>
     <row r="56">
@@ -981,10 +981,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>43882</v>
+        <v>43784</v>
       </c>
       <c r="C56" t="n">
-        <v>46.68</v>
+        <v>52.35</v>
       </c>
     </row>
     <row r="57">
@@ -992,10 +992,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>43885</v>
+        <v>43787</v>
       </c>
       <c r="C57" t="n">
-        <v>44.69</v>
+        <v>51.83</v>
       </c>
     </row>
     <row r="58">
@@ -1003,10 +1003,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>43886</v>
+        <v>43788</v>
       </c>
       <c r="C58" t="n">
-        <v>42.48</v>
+        <v>50.95</v>
       </c>
     </row>
     <row r="59">
@@ -1014,10 +1014,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>43887</v>
+        <v>43789</v>
       </c>
       <c r="C59" t="n">
-        <v>41.61</v>
+        <v>50.26</v>
       </c>
     </row>
     <row r="60">
@@ -1025,10 +1025,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>43888</v>
+        <v>43790</v>
       </c>
       <c r="C60" t="n">
-        <v>38.85</v>
+        <v>51.41</v>
       </c>
     </row>
     <row r="61">
@@ -1036,10 +1036,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>43889</v>
+        <v>43791</v>
       </c>
       <c r="C61" t="n">
-        <v>39.7</v>
+        <v>51.72</v>
       </c>
     </row>
     <row r="62">
@@ -1047,10 +1047,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>43892</v>
+        <v>43794</v>
       </c>
       <c r="C62" t="n">
-        <v>40.69</v>
+        <v>52.67</v>
       </c>
     </row>
     <row r="63">
@@ -1058,10 +1058,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>43893</v>
+        <v>43795</v>
       </c>
       <c r="C63" t="n">
-        <v>39.85</v>
+        <v>52.84</v>
       </c>
     </row>
     <row r="64">
@@ -1069,10 +1069,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>43894</v>
+        <v>43796</v>
       </c>
       <c r="C64" t="n">
-        <v>41.17</v>
+        <v>52.46</v>
       </c>
     </row>
     <row r="65">
@@ -1080,10 +1080,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>43895</v>
+        <v>43798</v>
       </c>
       <c r="C65" t="n">
-        <v>39.4</v>
+        <v>51.58</v>
       </c>
     </row>
     <row r="66">
@@ -1091,10 +1091,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>43896</v>
+        <v>43801</v>
       </c>
       <c r="C66" t="n">
-        <v>38.28</v>
+        <v>51.38</v>
       </c>
     </row>
     <row r="67">
@@ -1102,10 +1102,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>43899</v>
+        <v>43802</v>
       </c>
       <c r="C67" t="n">
-        <v>29.99</v>
+        <v>50.08</v>
       </c>
     </row>
     <row r="68">
@@ -1113,10 +1113,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>43900</v>
+        <v>43803</v>
       </c>
       <c r="C68" t="n">
-        <v>30.85</v>
+        <v>50.53</v>
       </c>
     </row>
     <row r="69">
@@ -1124,10 +1124,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>43901</v>
+        <v>43804</v>
       </c>
       <c r="C69" t="n">
-        <v>27.5</v>
+        <v>50.26</v>
       </c>
     </row>
     <row r="70">
@@ -1135,10 +1135,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>43902</v>
+        <v>43805</v>
       </c>
       <c r="C70" t="n">
-        <v>23.25</v>
+        <v>51.43</v>
       </c>
     </row>
     <row r="71">
@@ -1146,10 +1146,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>43903</v>
+        <v>43808</v>
       </c>
       <c r="C71" t="n">
-        <v>25.24</v>
+        <v>51.48</v>
       </c>
     </row>
     <row r="72">
@@ -1157,10 +1157,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>43906</v>
+        <v>43809</v>
       </c>
       <c r="C72" t="n">
-        <v>21.61</v>
+        <v>51.35</v>
       </c>
     </row>
     <row r="73">
@@ -1168,10 +1168,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>43907</v>
+        <v>43810</v>
       </c>
       <c r="C73" t="n">
-        <v>26.13</v>
+        <v>51.32</v>
       </c>
     </row>
     <row r="74">
@@ -1179,10 +1179,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>43908</v>
+        <v>43811</v>
       </c>
       <c r="C74" t="n">
-        <v>25.98</v>
+        <v>52.62</v>
       </c>
     </row>
     <row r="75">
@@ -1190,10 +1190,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>43909</v>
+        <v>43812</v>
       </c>
       <c r="C75" t="n">
-        <v>27.63</v>
+        <v>51.49</v>
       </c>
     </row>
     <row r="76">
@@ -1201,10 +1201,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>43910</v>
+        <v>43815</v>
       </c>
       <c r="C76" t="n">
-        <v>26.96</v>
+        <v>52.35</v>
       </c>
     </row>
     <row r="77">
@@ -1212,10 +1212,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>43913</v>
+        <v>43816</v>
       </c>
       <c r="C77" t="n">
-        <v>26.11</v>
+        <v>52.83</v>
       </c>
     </row>
     <row r="78">
@@ -1223,10 +1223,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>43914</v>
+        <v>43817</v>
       </c>
       <c r="C78" t="n">
-        <v>27.97</v>
+        <v>52.43</v>
       </c>
     </row>
     <row r="79">
@@ -1234,10 +1234,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>43915</v>
+        <v>43818</v>
       </c>
       <c r="C79" t="n">
-        <v>29.85</v>
+        <v>52.69</v>
       </c>
     </row>
     <row r="80">
@@ -1245,10 +1245,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="n">
-        <v>43916</v>
+        <v>43819</v>
       </c>
       <c r="C80" t="n">
-        <v>29.16</v>
+        <v>52.78</v>
       </c>
     </row>
     <row r="81">
@@ -1256,10 +1256,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="n">
-        <v>43917</v>
+        <v>43822</v>
       </c>
       <c r="C81" t="n">
-        <v>28.06</v>
+        <v>53.09</v>
       </c>
     </row>
     <row r="82">
@@ -1267,10 +1267,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="n">
-        <v>43920</v>
+        <v>43823</v>
       </c>
       <c r="C82" t="n">
-        <v>28.15</v>
+        <v>53.06</v>
       </c>
     </row>
     <row r="83">
@@ -1278,10 +1278,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="n">
-        <v>43921</v>
+        <v>43825</v>
       </c>
       <c r="C83" t="n">
-        <v>28.73</v>
+        <v>53.37</v>
       </c>
     </row>
     <row r="84">
@@ -1289,10 +1289,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="n">
-        <v>43922</v>
+        <v>43826</v>
       </c>
       <c r="C84" t="n">
-        <v>26.56</v>
+        <v>52.99</v>
       </c>
     </row>
     <row r="85">
@@ -1300,10 +1300,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="n">
-        <v>43923</v>
+        <v>43829</v>
       </c>
       <c r="C85" t="n">
-        <v>27.54</v>
+        <v>52.52</v>
       </c>
     </row>
     <row r="86">
@@ -1311,10 +1311,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="n">
-        <v>43924</v>
+        <v>43830</v>
       </c>
       <c r="C86" t="n">
-        <v>27.48</v>
+        <v>52.89</v>
       </c>
     </row>
     <row r="87">
@@ -1322,10 +1322,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="n">
-        <v>43927</v>
+        <v>43832</v>
       </c>
       <c r="C87" t="n">
-        <v>30</v>
+        <v>51.95</v>
       </c>
     </row>
     <row r="88">
@@ -1333,10 +1333,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="n">
-        <v>43928</v>
+        <v>43833</v>
       </c>
       <c r="C88" t="n">
-        <v>31.76</v>
+        <v>50.66</v>
       </c>
     </row>
     <row r="89">
@@ -1344,10 +1344,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="n">
-        <v>43929</v>
+        <v>43836</v>
       </c>
       <c r="C89" t="n">
-        <v>34.18</v>
+        <v>50.46</v>
       </c>
     </row>
     <row r="90">
@@ -1355,10 +1355,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="n">
-        <v>43930</v>
+        <v>43837</v>
       </c>
       <c r="C90" t="n">
-        <v>35.92</v>
+        <v>50.44</v>
       </c>
     </row>
     <row r="91">
@@ -1366,10 +1366,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="n">
-        <v>43934</v>
+        <v>43838</v>
       </c>
       <c r="C91" t="n">
-        <v>34.61</v>
+        <v>50.96</v>
       </c>
     </row>
     <row r="92">
@@ -1377,10 +1377,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="n">
-        <v>43935</v>
+        <v>43839</v>
       </c>
       <c r="C92" t="n">
-        <v>34.75</v>
+        <v>50.44</v>
       </c>
     </row>
     <row r="93">
@@ -1388,10 +1388,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="n">
-        <v>43936</v>
+        <v>43840</v>
       </c>
       <c r="C93" t="n">
-        <v>31.66</v>
+        <v>49.77</v>
       </c>
     </row>
     <row r="94">
@@ -1399,10 +1399,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="n">
-        <v>43937</v>
+        <v>43843</v>
       </c>
       <c r="C94" t="n">
-        <v>31.07</v>
+        <v>50.59</v>
       </c>
     </row>
     <row r="95">
@@ -1410,10 +1410,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="n">
-        <v>43938</v>
+        <v>43844</v>
       </c>
       <c r="C95" t="n">
-        <v>32.83</v>
+        <v>50.49</v>
       </c>
     </row>
     <row r="96">
@@ -1421,10 +1421,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="n">
-        <v>43941</v>
+        <v>43845</v>
       </c>
       <c r="C96" t="n">
-        <v>30.98</v>
+        <v>50.52</v>
       </c>
     </row>
     <row r="97">
@@ -1432,10 +1432,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="n">
-        <v>43942</v>
+        <v>43846</v>
       </c>
       <c r="C97" t="n">
-        <v>30.34</v>
+        <v>50.72</v>
       </c>
     </row>
     <row r="98">
@@ -1443,10 +1443,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="n">
-        <v>43943</v>
+        <v>43847</v>
       </c>
       <c r="C98" t="n">
-        <v>31.28</v>
+        <v>51.55</v>
       </c>
     </row>
     <row r="99">
@@ -1454,10 +1454,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="n">
-        <v>43944</v>
+        <v>43851</v>
       </c>
       <c r="C99" t="n">
-        <v>31.99</v>
+        <v>50.84</v>
       </c>
     </row>
     <row r="100">
@@ -1465,10 +1465,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="n">
-        <v>43945</v>
+        <v>43852</v>
       </c>
       <c r="C100" t="n">
-        <v>32.54</v>
+        <v>49.16</v>
       </c>
     </row>
     <row r="101">
@@ -1476,10 +1476,10 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="n">
-        <v>43948</v>
+        <v>43853</v>
       </c>
       <c r="C101" t="n">
-        <v>33.83</v>
+        <v>48.56</v>
       </c>
     </row>
     <row r="102">
@@ -1487,10 +1487,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="n">
-        <v>43949</v>
+        <v>43854</v>
       </c>
       <c r="C102" t="n">
-        <v>35.24</v>
+        <v>46.86</v>
       </c>
     </row>
     <row r="103">
@@ -1498,10 +1498,10 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="n">
-        <v>43950</v>
+        <v>43857</v>
       </c>
       <c r="C103" t="n">
-        <v>36.81</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="104">
@@ -1509,10 +1509,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="n">
-        <v>43951</v>
+        <v>43858</v>
       </c>
       <c r="C104" t="n">
-        <v>36.05</v>
+        <v>45.58</v>
       </c>
     </row>
     <row r="105">
@@ -1520,10 +1520,10 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="n">
-        <v>43952</v>
+        <v>43859</v>
       </c>
       <c r="C105" t="n">
-        <v>33.33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106">
@@ -1531,10 +1531,10 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="n">
-        <v>43955</v>
+        <v>43860</v>
       </c>
       <c r="C106" t="n">
-        <v>32.48</v>
+        <v>46.84</v>
       </c>
     </row>
     <row r="107">
@@ -1542,10 +1542,10 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="n">
-        <v>43956</v>
+        <v>43861</v>
       </c>
       <c r="C107" t="n">
-        <v>32.78</v>
+        <v>44.52</v>
       </c>
     </row>
     <row r="108">
@@ -1553,10 +1553,10 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="n">
-        <v>43957</v>
+        <v>43864</v>
       </c>
       <c r="C108" t="n">
-        <v>31.4</v>
+        <v>45.17</v>
       </c>
     </row>
     <row r="109">
@@ -1564,10 +1564,10 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="n">
-        <v>43958</v>
+        <v>43865</v>
       </c>
       <c r="C109" t="n">
-        <v>32.27</v>
+        <v>46.44</v>
       </c>
     </row>
     <row r="110">
@@ -1575,10 +1575,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="n">
-        <v>43959</v>
+        <v>43866</v>
       </c>
       <c r="C110" t="n">
-        <v>33.73</v>
+        <v>47.95</v>
       </c>
     </row>
     <row r="111">
@@ -1586,10 +1586,10 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="n">
-        <v>43962</v>
+        <v>43867</v>
       </c>
       <c r="C111" t="n">
-        <v>33.3</v>
+        <v>47.55</v>
       </c>
     </row>
     <row r="112">
@@ -1597,10 +1597,10 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="n">
-        <v>43963</v>
+        <v>43868</v>
       </c>
       <c r="C112" t="n">
-        <v>33.2</v>
+        <v>46.42</v>
       </c>
     </row>
     <row r="113">
@@ -1608,10 +1608,10 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="n">
-        <v>43964</v>
+        <v>43871</v>
       </c>
       <c r="C113" t="n">
-        <v>31.78</v>
+        <v>46.57</v>
       </c>
     </row>
     <row r="114">
@@ -1619,10 +1619,10 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="n">
-        <v>43965</v>
+        <v>43872</v>
       </c>
       <c r="C114" t="n">
-        <v>32.92</v>
+        <v>47.15</v>
       </c>
     </row>
     <row r="115">
@@ -1630,10 +1630,10 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="n">
-        <v>43966</v>
+        <v>43873</v>
       </c>
       <c r="C115" t="n">
-        <v>32.97</v>
+        <v>47.72</v>
       </c>
     </row>
     <row r="116">
@@ -1641,10 +1641,10 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="n">
-        <v>43969</v>
+        <v>43874</v>
       </c>
       <c r="C116" t="n">
-        <v>36.09</v>
+        <v>46.68</v>
       </c>
     </row>
     <row r="117">
@@ -1652,10 +1652,10 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="n">
-        <v>43970</v>
+        <v>43875</v>
       </c>
       <c r="C117" t="n">
-        <v>35.01</v>
+        <v>47</v>
       </c>
     </row>
     <row r="118">
@@ -1663,10 +1663,10 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="n">
-        <v>43971</v>
+        <v>43879</v>
       </c>
       <c r="C118" t="n">
-        <v>35.54</v>
+        <v>46.14</v>
       </c>
     </row>
     <row r="119">
@@ -1674,10 +1674,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="n">
-        <v>43972</v>
+        <v>43880</v>
       </c>
       <c r="C119" t="n">
-        <v>35.19</v>
+        <v>45.96</v>
       </c>
     </row>
     <row r="120">
@@ -1685,10 +1685,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="n">
-        <v>43973</v>
+        <v>43881</v>
       </c>
       <c r="C120" t="n">
-        <v>35.49</v>
+        <v>47.12</v>
       </c>
     </row>
     <row r="121">
@@ -1696,10 +1696,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="n">
-        <v>43977</v>
+        <v>43882</v>
       </c>
       <c r="C121" t="n">
-        <v>38.11</v>
+        <v>46.68</v>
       </c>
     </row>
     <row r="122">
@@ -1707,10 +1707,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="n">
-        <v>43978</v>
+        <v>43885</v>
       </c>
       <c r="C122" t="n">
-        <v>39.12</v>
+        <v>44.69</v>
       </c>
     </row>
     <row r="123">
@@ -1718,10 +1718,10 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="n">
-        <v>43979</v>
+        <v>43886</v>
       </c>
       <c r="C123" t="n">
-        <v>38.71</v>
+        <v>42.48</v>
       </c>
     </row>
     <row r="124">
@@ -1729,10 +1729,10 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="n">
-        <v>43980</v>
+        <v>43887</v>
       </c>
       <c r="C124" t="n">
-        <v>38.6</v>
+        <v>41.61</v>
       </c>
     </row>
     <row r="125">
@@ -1740,10 +1740,10 @@
         <v>123</v>
       </c>
       <c r="B125" s="2" t="n">
-        <v>43983</v>
+        <v>43888</v>
       </c>
       <c r="C125" t="n">
-        <v>38.61</v>
+        <v>38.85</v>
       </c>
     </row>
     <row r="126">
@@ -1751,10 +1751,10 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="n">
-        <v>43984</v>
+        <v>43889</v>
       </c>
       <c r="C126" t="n">
-        <v>40.6</v>
+        <v>39.7</v>
       </c>
     </row>
     <row r="127">
@@ -1762,10 +1762,10 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="n">
-        <v>43985</v>
+        <v>43892</v>
       </c>
       <c r="C127" t="n">
-        <v>41.63</v>
+        <v>40.69</v>
       </c>
     </row>
     <row r="128">
@@ -1773,10 +1773,10 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="n">
-        <v>43986</v>
+        <v>43893</v>
       </c>
       <c r="C128" t="n">
-        <v>42.71</v>
+        <v>39.85</v>
       </c>
     </row>
     <row r="129">
@@ -1784,10 +1784,10 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="n">
-        <v>43987</v>
+        <v>43894</v>
       </c>
       <c r="C129" t="n">
-        <v>43.97</v>
+        <v>41.17</v>
       </c>
     </row>
     <row r="130">
@@ -1795,10 +1795,10 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="n">
-        <v>43990</v>
+        <v>43895</v>
       </c>
       <c r="C130" t="n">
-        <v>45.9</v>
+        <v>39.4</v>
       </c>
     </row>
     <row r="131">
@@ -1806,10 +1806,10 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="n">
-        <v>43991</v>
+        <v>43896</v>
       </c>
       <c r="C131" t="n">
-        <v>44.41</v>
+        <v>38.28</v>
       </c>
     </row>
     <row r="132">
@@ -1817,10 +1817,10 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="n">
-        <v>43992</v>
+        <v>43899</v>
       </c>
       <c r="C132" t="n">
-        <v>43.58</v>
+        <v>29.99</v>
       </c>
     </row>
     <row r="133">
@@ -1828,10 +1828,10 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="n">
-        <v>43993</v>
+        <v>43900</v>
       </c>
       <c r="C133" t="n">
-        <v>39.26</v>
+        <v>30.85</v>
       </c>
     </row>
     <row r="134">
@@ -1839,10 +1839,10 @@
         <v>132</v>
       </c>
       <c r="B134" s="2" t="n">
-        <v>43994</v>
+        <v>43901</v>
       </c>
       <c r="C134" t="n">
-        <v>41.23</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="135">
@@ -1850,10 +1850,10 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="n">
-        <v>43997</v>
+        <v>43902</v>
       </c>
       <c r="C135" t="n">
-        <v>41.98</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="136">
@@ -1861,10 +1861,10 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="n">
-        <v>43998</v>
+        <v>43903</v>
       </c>
       <c r="C136" t="n">
-        <v>42.25</v>
+        <v>25.24</v>
       </c>
     </row>
     <row r="137">
@@ -1872,10 +1872,10 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="n">
-        <v>43999</v>
+        <v>43906</v>
       </c>
       <c r="C137" t="n">
-        <v>41.17</v>
+        <v>21.61</v>
       </c>
     </row>
     <row r="138">
@@ -1883,10 +1883,10 @@
         <v>136</v>
       </c>
       <c r="B138" s="2" t="n">
-        <v>44000</v>
+        <v>43907</v>
       </c>
       <c r="C138" t="n">
-        <v>41.58</v>
+        <v>26.13</v>
       </c>
     </row>
     <row r="139">
@@ -1894,10 +1894,10 @@
         <v>137</v>
       </c>
       <c r="B139" s="2" t="n">
-        <v>44001</v>
+        <v>43908</v>
       </c>
       <c r="C139" t="n">
-        <v>41.65</v>
+        <v>25.98</v>
       </c>
     </row>
     <row r="140">
@@ -1905,10 +1905,10 @@
         <v>138</v>
       </c>
       <c r="B140" s="2" t="n">
-        <v>44004</v>
+        <v>43909</v>
       </c>
       <c r="C140" t="n">
-        <v>41.74</v>
+        <v>27.63</v>
       </c>
     </row>
     <row r="141">
@@ -1916,10 +1916,10 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="n">
-        <v>44005</v>
+        <v>43910</v>
       </c>
       <c r="C141" t="n">
-        <v>41.35</v>
+        <v>26.96</v>
       </c>
     </row>
     <row r="142">
@@ -1927,10 +1927,10 @@
         <v>140</v>
       </c>
       <c r="B142" s="2" t="n">
-        <v>44006</v>
+        <v>43913</v>
       </c>
       <c r="C142" t="n">
-        <v>38.45</v>
+        <v>26.11</v>
       </c>
     </row>
     <row r="143">
@@ -1938,10 +1938,10 @@
         <v>141</v>
       </c>
       <c r="B143" s="2" t="n">
-        <v>44007</v>
+        <v>43914</v>
       </c>
       <c r="C143" t="n">
-        <v>39.98</v>
+        <v>27.97</v>
       </c>
     </row>
     <row r="144">
@@ -1949,10 +1949,10 @@
         <v>142</v>
       </c>
       <c r="B144" s="2" t="n">
-        <v>44008</v>
+        <v>43915</v>
       </c>
       <c r="C144" t="n">
-        <v>39.8</v>
+        <v>29.85</v>
       </c>
     </row>
     <row r="145">
@@ -1960,10 +1960,10 @@
         <v>143</v>
       </c>
       <c r="B145" s="2" t="n">
-        <v>44011</v>
+        <v>43916</v>
       </c>
       <c r="C145" t="n">
-        <v>40.98</v>
+        <v>29.16</v>
       </c>
     </row>
     <row r="146">
@@ -1971,10 +1971,10 @@
         <v>144</v>
       </c>
       <c r="B146" s="2" t="n">
-        <v>44012</v>
+        <v>43917</v>
       </c>
       <c r="C146" t="n">
-        <v>40.76</v>
+        <v>28.06</v>
       </c>
     </row>
     <row r="147">
@@ -1982,10 +1982,10 @@
         <v>145</v>
       </c>
       <c r="B147" s="2" t="n">
-        <v>44013</v>
+        <v>43920</v>
       </c>
       <c r="C147" t="n">
-        <v>40.75</v>
+        <v>28.15</v>
       </c>
     </row>
     <row r="148">
@@ -1993,10 +1993,10 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="n">
-        <v>44014</v>
+        <v>43921</v>
       </c>
       <c r="C148" t="n">
-        <v>41.59</v>
+        <v>28.73</v>
       </c>
     </row>
     <row r="149">
@@ -2004,10 +2004,10 @@
         <v>147</v>
       </c>
       <c r="B149" s="2" t="n">
-        <v>44018</v>
+        <v>43922</v>
       </c>
       <c r="C149" t="n">
-        <v>42.45</v>
+        <v>26.56</v>
       </c>
     </row>
     <row r="150">
@@ -2015,10 +2015,10 @@
         <v>148</v>
       </c>
       <c r="B150" s="2" t="n">
-        <v>44019</v>
+        <v>43923</v>
       </c>
       <c r="C150" t="n">
-        <v>41.69</v>
+        <v>27.54</v>
       </c>
     </row>
     <row r="151">
@@ -2026,10 +2026,10 @@
         <v>149</v>
       </c>
       <c r="B151" s="2" t="n">
-        <v>44020</v>
+        <v>43924</v>
       </c>
       <c r="C151" t="n">
-        <v>40.35</v>
+        <v>27.48</v>
       </c>
     </row>
     <row r="152">
@@ -2037,10 +2037,10 @@
         <v>150</v>
       </c>
       <c r="B152" s="2" t="n">
-        <v>44021</v>
+        <v>43927</v>
       </c>
       <c r="C152" t="n">
-        <v>39.44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153">
@@ -2048,10 +2048,10 @@
         <v>151</v>
       </c>
       <c r="B153" s="2" t="n">
-        <v>44022</v>
+        <v>43928</v>
       </c>
       <c r="C153" t="n">
-        <v>40.76</v>
+        <v>31.76</v>
       </c>
     </row>
     <row r="154">
@@ -2059,10 +2059,10 @@
         <v>152</v>
       </c>
       <c r="B154" s="2" t="n">
-        <v>44025</v>
+        <v>43929</v>
       </c>
       <c r="C154" t="n">
-        <v>41.24</v>
+        <v>34.18</v>
       </c>
     </row>
     <row r="155">
@@ -2070,10 +2070,10 @@
         <v>153</v>
       </c>
       <c r="B155" s="2" t="n">
-        <v>44026</v>
+        <v>43930</v>
       </c>
       <c r="C155" t="n">
-        <v>42.44</v>
+        <v>35.92</v>
       </c>
     </row>
     <row r="156">
@@ -2081,10 +2081,10 @@
         <v>154</v>
       </c>
       <c r="B156" s="2" t="n">
-        <v>44027</v>
+        <v>43934</v>
       </c>
       <c r="C156" t="n">
-        <v>43.33</v>
+        <v>34.61</v>
       </c>
     </row>
     <row r="157">
@@ -2092,10 +2092,10 @@
         <v>155</v>
       </c>
       <c r="B157" s="2" t="n">
-        <v>44028</v>
+        <v>43935</v>
       </c>
       <c r="C157" t="n">
-        <v>43.83</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="158">
@@ -2103,10 +2103,10 @@
         <v>156</v>
       </c>
       <c r="B158" s="2" t="n">
-        <v>44029</v>
+        <v>43936</v>
       </c>
       <c r="C158" t="n">
-        <v>43.67</v>
+        <v>31.66</v>
       </c>
     </row>
     <row r="159">
@@ -2114,10 +2114,10 @@
         <v>157</v>
       </c>
       <c r="B159" s="2" t="n">
-        <v>44032</v>
+        <v>43937</v>
       </c>
       <c r="C159" t="n">
-        <v>42.3</v>
+        <v>31.07</v>
       </c>
     </row>
     <row r="160">
@@ -2125,10 +2125,10 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="n">
-        <v>44033</v>
+        <v>43938</v>
       </c>
       <c r="C160" t="n">
-        <v>43.04</v>
+        <v>32.83</v>
       </c>
     </row>
     <row r="161">
@@ -2136,10 +2136,10 @@
         <v>159</v>
       </c>
       <c r="B161" s="2" t="n">
-        <v>44034</v>
+        <v>43941</v>
       </c>
       <c r="C161" t="n">
-        <v>44.34</v>
+        <v>30.98</v>
       </c>
     </row>
     <row r="162">
@@ -2147,10 +2147,10 @@
         <v>160</v>
       </c>
       <c r="B162" s="2" t="n">
-        <v>44035</v>
+        <v>43942</v>
       </c>
       <c r="C162" t="n">
-        <v>42.82</v>
+        <v>30.34</v>
       </c>
     </row>
     <row r="163">
@@ -2158,10 +2158,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="2" t="n">
-        <v>44036</v>
+        <v>43943</v>
       </c>
       <c r="C163" t="n">
-        <v>42.61</v>
+        <v>31.28</v>
       </c>
     </row>
     <row r="164">
@@ -2169,10 +2169,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="2" t="n">
-        <v>44039</v>
+        <v>43944</v>
       </c>
       <c r="C164" t="n">
-        <v>44</v>
+        <v>31.99</v>
       </c>
     </row>
     <row r="165">
@@ -2180,10 +2180,10 @@
         <v>163</v>
       </c>
       <c r="B165" s="2" t="n">
-        <v>44040</v>
+        <v>43945</v>
       </c>
       <c r="C165" t="n">
-        <v>42.62</v>
+        <v>32.54</v>
       </c>
     </row>
     <row r="166">
@@ -2191,10 +2191,10 @@
         <v>164</v>
       </c>
       <c r="B166" s="2" t="n">
-        <v>44041</v>
+        <v>43948</v>
       </c>
       <c r="C166" t="n">
-        <v>43.52</v>
+        <v>33.83</v>
       </c>
     </row>
     <row r="167">
@@ -2202,10 +2202,10 @@
         <v>165</v>
       </c>
       <c r="B167" s="2" t="n">
-        <v>44042</v>
+        <v>43949</v>
       </c>
       <c r="C167" t="n">
-        <v>41.73</v>
+        <v>35.24</v>
       </c>
     </row>
     <row r="168">
@@ -2213,10 +2213,780 @@
         <v>166</v>
       </c>
       <c r="B168" s="2" t="n">
+        <v>43950</v>
+      </c>
+      <c r="C168" t="n">
+        <v>36.81</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" s="2" t="n">
+        <v>43951</v>
+      </c>
+      <c r="C169" t="n">
+        <v>36.05</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" s="2" t="n">
+        <v>43952</v>
+      </c>
+      <c r="C170" t="n">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" s="2" t="n">
+        <v>43955</v>
+      </c>
+      <c r="C171" t="n">
+        <v>32.48</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" s="2" t="n">
+        <v>43956</v>
+      </c>
+      <c r="C172" t="n">
+        <v>32.78</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" s="2" t="n">
+        <v>43957</v>
+      </c>
+      <c r="C173" t="n">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" s="2" t="n">
+        <v>43958</v>
+      </c>
+      <c r="C174" t="n">
+        <v>32.27</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" s="2" t="n">
+        <v>43959</v>
+      </c>
+      <c r="C175" t="n">
+        <v>33.73</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" s="2" t="n">
+        <v>43962</v>
+      </c>
+      <c r="C176" t="n">
+        <v>33.3</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" s="2" t="n">
+        <v>43963</v>
+      </c>
+      <c r="C177" t="n">
+        <v>33.2</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" s="2" t="n">
+        <v>43964</v>
+      </c>
+      <c r="C178" t="n">
+        <v>31.78</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" s="2" t="n">
+        <v>43965</v>
+      </c>
+      <c r="C179" t="n">
+        <v>32.92</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" s="2" t="n">
+        <v>43966</v>
+      </c>
+      <c r="C180" t="n">
+        <v>32.97</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" s="2" t="n">
+        <v>43969</v>
+      </c>
+      <c r="C181" t="n">
+        <v>36.09</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" s="2" t="n">
+        <v>43970</v>
+      </c>
+      <c r="C182" t="n">
+        <v>35.01</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" s="2" t="n">
+        <v>43971</v>
+      </c>
+      <c r="C183" t="n">
+        <v>35.54</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" s="2" t="n">
+        <v>43972</v>
+      </c>
+      <c r="C184" t="n">
+        <v>35.19</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" s="2" t="n">
+        <v>43973</v>
+      </c>
+      <c r="C185" t="n">
+        <v>35.49</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" s="2" t="n">
+        <v>43977</v>
+      </c>
+      <c r="C186" t="n">
+        <v>38.11</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" s="2" t="n">
+        <v>43978</v>
+      </c>
+      <c r="C187" t="n">
+        <v>39.12</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" s="2" t="n">
+        <v>43979</v>
+      </c>
+      <c r="C188" t="n">
+        <v>38.71</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" s="2" t="n">
+        <v>43980</v>
+      </c>
+      <c r="C189" t="n">
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" s="2" t="n">
+        <v>43983</v>
+      </c>
+      <c r="C190" t="n">
+        <v>38.61</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" s="2" t="n">
+        <v>43984</v>
+      </c>
+      <c r="C191" t="n">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" s="2" t="n">
+        <v>43985</v>
+      </c>
+      <c r="C192" t="n">
+        <v>41.63</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" s="2" t="n">
+        <v>43986</v>
+      </c>
+      <c r="C193" t="n">
+        <v>42.71</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" s="2" t="n">
+        <v>43987</v>
+      </c>
+      <c r="C194" t="n">
+        <v>43.97</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" s="2" t="n">
+        <v>43990</v>
+      </c>
+      <c r="C195" t="n">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" s="2" t="n">
+        <v>43991</v>
+      </c>
+      <c r="C196" t="n">
+        <v>44.41</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" s="2" t="n">
+        <v>43992</v>
+      </c>
+      <c r="C197" t="n">
+        <v>43.58</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" s="2" t="n">
+        <v>43993</v>
+      </c>
+      <c r="C198" t="n">
+        <v>39.26</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" s="2" t="n">
+        <v>43994</v>
+      </c>
+      <c r="C199" t="n">
+        <v>41.23</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" s="2" t="n">
+        <v>43997</v>
+      </c>
+      <c r="C200" t="n">
+        <v>41.98</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" s="2" t="n">
+        <v>43998</v>
+      </c>
+      <c r="C201" t="n">
+        <v>42.25</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" s="2" t="n">
+        <v>43999</v>
+      </c>
+      <c r="C202" t="n">
+        <v>41.17</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" s="2" t="n">
+        <v>44000</v>
+      </c>
+      <c r="C203" t="n">
+        <v>41.58</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" s="2" t="n">
+        <v>44001</v>
+      </c>
+      <c r="C204" t="n">
+        <v>41.65</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" s="2" t="n">
+        <v>44004</v>
+      </c>
+      <c r="C205" t="n">
+        <v>41.74</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" s="2" t="n">
+        <v>44005</v>
+      </c>
+      <c r="C206" t="n">
+        <v>41.35</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" s="2" t="n">
+        <v>44006</v>
+      </c>
+      <c r="C207" t="n">
+        <v>38.45</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" s="2" t="n">
+        <v>44007</v>
+      </c>
+      <c r="C208" t="n">
+        <v>39.98</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" s="2" t="n">
+        <v>44008</v>
+      </c>
+      <c r="C209" t="n">
+        <v>39.8</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" s="2" t="n">
+        <v>44011</v>
+      </c>
+      <c r="C210" t="n">
+        <v>40.98</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" s="2" t="n">
+        <v>44012</v>
+      </c>
+      <c r="C211" t="n">
+        <v>40.76</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" s="2" t="n">
+        <v>44013</v>
+      </c>
+      <c r="C212" t="n">
+        <v>40.75</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C213" t="n">
+        <v>41.59</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" s="2" t="n">
+        <v>44018</v>
+      </c>
+      <c r="C214" t="n">
+        <v>42.45</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C215" t="n">
+        <v>41.69</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C216" t="n">
+        <v>40.35</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" s="2" t="n">
+        <v>44021</v>
+      </c>
+      <c r="C217" t="n">
+        <v>39.44</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" s="2" t="n">
+        <v>44022</v>
+      </c>
+      <c r="C218" t="n">
+        <v>40.76</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" s="2" t="n">
+        <v>44025</v>
+      </c>
+      <c r="C219" t="n">
+        <v>41.24</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" s="2" t="n">
+        <v>44026</v>
+      </c>
+      <c r="C220" t="n">
+        <v>42.44</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" s="2" t="n">
+        <v>44027</v>
+      </c>
+      <c r="C221" t="n">
+        <v>43.33</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" s="2" t="n">
+        <v>44028</v>
+      </c>
+      <c r="C222" t="n">
+        <v>43.83</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" s="2" t="n">
+        <v>44029</v>
+      </c>
+      <c r="C223" t="n">
+        <v>43.67</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" s="2" t="n">
+        <v>44032</v>
+      </c>
+      <c r="C224" t="n">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" s="2" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C225" t="n">
+        <v>43.04</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C226" t="n">
+        <v>44.34</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C227" t="n">
+        <v>42.82</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" s="2" t="n">
+        <v>44036</v>
+      </c>
+      <c r="C228" t="n">
+        <v>42.61</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" s="2" t="n">
+        <v>44039</v>
+      </c>
+      <c r="C229" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C230" t="n">
+        <v>42.62</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C231" t="n">
+        <v>43.52</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" s="2" t="n">
+        <v>44042</v>
+      </c>
+      <c r="C232" t="n">
+        <v>41.73</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" s="2" t="n">
         <v>44043</v>
       </c>
-      <c r="C168" t="n">
+      <c r="C233" t="n">
         <v>41.06</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" s="2" t="n">
+        <v>44046</v>
+      </c>
+      <c r="C234" t="n">
+        <v>40.09</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" s="2" t="n">
+        <v>44047</v>
+      </c>
+      <c r="C235" t="n">
+        <v>41.32</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" s="2" t="n">
+        <v>44048</v>
+      </c>
+      <c r="C236" t="n">
+        <v>41.99</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" s="2" t="n">
+        <v>44049</v>
+      </c>
+      <c r="C237" t="n">
+        <v>42.05</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" s="2" t="n">
+        <v>44050</v>
+      </c>
+      <c r="C238" t="n">
+        <v>42.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>